<commit_message>
Model fitting based on data preprocessing
</commit_message>
<xml_diff>
--- a/out/img/core/BR_116_training_testing_data.xlsx
+++ b/out/img/core/BR_116_training_testing_data.xlsx
@@ -509,11 +509,7 @@
       <c r="C2" t="n">
         <v>86</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1,00999,00766,00343,00489,00812,0080,004,0098,005675,0051,0016,000,00963,00760,00244,00652,00967,00155,006,00143,005598,0052,0025,00</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -527,11 +523,7 @@
       <c r="C3" t="n">
         <v>71</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>0,006647,004853,002299,003150,005097,00612,0014,00617,0033883,00289,0062,002,006283,004941,001582,003612,005364,00736,0045,00902,0034152,00323,00102,00</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -545,11 +537,7 @@
       <c r="C4" t="n">
         <v>96</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2,006392,005013,002351,003206,005142,00754,0028,00685,0040617,00251,0062,000,006077,005251,001357,003632,005341,00795,0049,00740,0047979,00330,0088,00</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>